<commit_message>
update data and true_create_graph
</commit_message>
<xml_diff>
--- a/data/insomnia_and_sleep_quality_relation.xlsx
+++ b/data/insomnia_and_sleep_quality_relation.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\87236\Projects\SR_ZJUPH_KnowledgeGraph\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60B6B15-FCED-4285-A45D-5EAEC2D036E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94592CCF-7F45-4314-8242-360389FFD0B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9420" xr2:uid="{A74AF67B-B8DE-324A-8CF4-54C0E0FA910C}"/>
+    <workbookView xWindow="12672" yWindow="1668" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{A74AF67B-B8DE-324A-8CF4-54C0E0FA910C}"/>
   </bookViews>
   <sheets>
     <sheet name="RELATION" sheetId="2" r:id="rId1"/>
+    <sheet name="EN_RELATION" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Relation</t>
   </si>
@@ -49,6 +50,12 @@
   </si>
   <si>
     <t>CLASSIFICATION</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>Subject</t>
   </si>
 </sst>
 </file>
@@ -448,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E22939-B604-E743-97A1-7B1F610CA2E1}">
   <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -754,4 +761,30 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61A69D4-AD73-4648-BC87-F647DE9BEF30}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>